<commit_message>
commit add them ki nang song
</commit_message>
<xml_diff>
--- a/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-trainghiemsangtao.xlsx
+++ b/TraiNghiemSangTao/TraiNghiemSangTao/Utils/Files/ds-trainghiemsangtao.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>DANH SÁCH TRẢI NGHIỆM SÁNG TẠO</t>
   </si>
@@ -20,7 +20,7 @@
     <t>TIẾT HỌC NGOÀI TRỜI TẠI THẢO CẦM VIÊN</t>
   </si>
   <si>
-    <t>Từ ngày 13/07/2018 tới ngày 13/08/2018</t>
+    <t>Từ ngày 18/07/2018 tới ngày 18/08/2018</t>
   </si>
   <si>
     <t>STT</t>
@@ -62,52 +62,49 @@
     <t>EMAIL</t>
   </si>
   <si>
+    <t>THCS Lê Lợi</t>
+  </si>
+  <si>
+    <t>Lớp 8</t>
+  </si>
+  <si>
+    <t>25/07/2018</t>
+  </si>
+  <si>
+    <t>Buổi sáng</t>
+  </si>
+  <si>
+    <t>Tiết học ngoài trời tại Thảo Cầm Viên</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>06/07/2018</t>
+  </si>
+  <si>
+    <t>Thành Trương Hữu</t>
+  </si>
+  <si>
+    <t>Hiệu Trưởng</t>
+  </si>
+  <si>
+    <t>988670449</t>
+  </si>
+  <si>
+    <t>truonghuuthanh95@gmail.com</t>
+  </si>
+  <si>
     <t>TH Hoà Bình</t>
   </si>
   <si>
     <t>Lớp 1</t>
   </si>
   <si>
-    <t>14/07/2018</t>
-  </si>
-  <si>
-    <t>Buổi sáng</t>
-  </si>
-  <si>
-    <t>Tiết học ngoài trời tại Thảo Cầm Viên</t>
-  </si>
-  <si>
-    <t>abc</t>
+    <t>26/07/2018</t>
   </si>
   <si>
     <t>04/07/2018</t>
-  </si>
-  <si>
-    <t>Thành Trương Hữu</t>
-  </si>
-  <si>
-    <t>Hiệu Trưởng</t>
-  </si>
-  <si>
-    <t>988670449</t>
-  </si>
-  <si>
-    <t>truonghuuthanh95@gmail.com</t>
-  </si>
-  <si>
-    <t>THCS Lê Lợi</t>
-  </si>
-  <si>
-    <t>Lớp 8</t>
-  </si>
-  <si>
-    <t>25/07/2018</t>
-  </si>
-  <si>
-    <t>06/07/2018</t>
-  </si>
-  <si>
-    <t>26/07/2018</t>
   </si>
 </sst>
 </file>
@@ -183,7 +180,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:M9"/>
+  <dimension ref="A2:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -336,7 +333,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="0">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>29</v>
@@ -363,47 +360,6 @@
         <v>25</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="0">
-        <v>80</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="0" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>